<commit_message>
update readme and download template
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19470" windowHeight="6000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12030" windowHeight="2685"/>
   </bookViews>
   <sheets>
     <sheet name="指示者信息" sheetId="1" r:id="rId1"/>
     <sheet name="指示者关系人员" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N20"/>
+  <oleSize ref="A1:H6"/>
 </workbook>
 </file>
 
@@ -491,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
@@ -569,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>

</xml_diff>